<commit_message>
Add error upon no container number specified
</commit_message>
<xml_diff>
--- a/server_files/test_data_2 - Copy.xlsx
+++ b/server_files/test_data_2 - Copy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LG4000\Desktop\comms\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4094FE00-E0CF-48FB-BB82-DBDBC51776AD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F45BCA-EEDE-4F10-87B5-AEB813162ED3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B3B8992A-2509-491A-9C39-2580EA4D3B1D}"/>
   </bookViews>
@@ -654,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CEAC2C5-08A0-40A6-93E9-BE2759C1F504}">
   <dimension ref="A1:Y147"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="121" workbookViewId="0">
-      <selection activeCell="E4" sqref="E2:E4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="121" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>